<commit_message>
1654 case with 30 connections faces convergence issue
</commit_message>
<xml_diff>
--- a/casefile_test_record/casefile_test.xlsx
+++ b/casefile_test_record/casefile_test.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="112">
   <si>
     <t>Region</t>
   </si>
@@ -332,6 +332,36 @@
   </si>
   <si>
     <t>1654-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1-106</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2-77</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2-164</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1-164</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1-822</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2-220</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1-1254</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2-248</t>
+  </si>
+  <si>
+    <t>1-1335</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2-258</t>
   </si>
 </sst>
 </file>
@@ -3727,8 +3757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U298" workbookViewId="0">
-      <selection activeCell="AH340" sqref="AH340"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AA31" sqref="AA31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4695,6 +4725,9 @@
       <c r="AC21" s="1">
         <v>106</v>
       </c>
+      <c r="AD21" s="25" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="34"/>
@@ -9267,6 +9300,9 @@
       <c r="AC126" s="1">
         <v>627</v>
       </c>
+      <c r="AD126" s="25" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="127" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A127" s="34"/>
@@ -10732,7 +10768,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="161" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A161" s="34"/>
       <c r="B161" s="1">
         <v>810</v>
@@ -10774,7 +10810,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="162" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A162" s="34"/>
       <c r="B162" s="1">
         <v>811</v>
@@ -10816,7 +10852,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="163" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A163" s="34"/>
       <c r="B163" s="1">
         <v>812</v>
@@ -10858,7 +10894,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="164" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A164" s="34"/>
       <c r="B164" s="22">
         <v>813</v>
@@ -10900,7 +10936,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="165" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A165" s="34"/>
       <c r="B165" s="1">
         <v>819</v>
@@ -10942,7 +10978,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="166" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A166" s="34"/>
       <c r="B166" s="1">
         <v>820</v>
@@ -10984,7 +11020,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="167" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A167" s="34"/>
       <c r="B167" s="1">
         <v>822</v>
@@ -11025,8 +11061,11 @@
       <c r="AC167" s="1">
         <v>822</v>
       </c>
-    </row>
-    <row r="168" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD167" s="25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="168" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A168" s="34"/>
       <c r="B168" s="1">
         <v>836</v>
@@ -11068,7 +11107,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="169" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A169" s="34"/>
       <c r="B169" s="1">
         <v>837</v>
@@ -11110,7 +11149,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="170" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A170" s="34"/>
       <c r="B170" s="1">
         <v>844</v>
@@ -11152,7 +11191,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="171" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A171" s="34"/>
       <c r="B171" s="22">
         <v>853</v>
@@ -11194,7 +11233,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="172" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A172" s="34"/>
       <c r="B172" s="1">
         <v>857</v>
@@ -11236,7 +11275,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="173" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A173" s="34"/>
       <c r="B173" s="1">
         <v>861</v>
@@ -11278,7 +11317,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="174" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A174" s="34"/>
       <c r="B174" s="1">
         <v>863</v>
@@ -11320,7 +11359,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="175" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A175" s="34"/>
       <c r="B175" s="1">
         <v>869</v>
@@ -11362,7 +11401,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="176" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A176" s="34"/>
       <c r="B176" s="22">
         <v>872</v>
@@ -14271,6 +14310,9 @@
       <c r="AC242" s="1">
         <v>1254</v>
       </c>
+      <c r="AD242" s="25" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="243" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A243" s="34"/>
@@ -14931,6 +14973,9 @@
       <c r="AC257" s="1">
         <v>1335</v>
       </c>
+      <c r="AD257" s="25" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="258" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A258" s="34"/>
@@ -15551,6 +15596,9 @@
       <c r="AC269">
         <v>77</v>
       </c>
+      <c r="AD269" s="25" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="270" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A270" s="34"/>
@@ -16451,6 +16499,9 @@
       <c r="AC288" s="1">
         <v>164</v>
       </c>
+      <c r="AD288" s="25" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="289" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A289" s="34"/>
@@ -17195,6 +17246,9 @@
       <c r="AC304">
         <v>220</v>
       </c>
+      <c r="AD304" s="25" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="305" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A305" s="34"/>
@@ -17375,6 +17429,9 @@
       <c r="AC308" s="1">
         <v>248</v>
       </c>
+      <c r="AD308" s="25" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="309" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A309" s="34"/>
@@ -17831,6 +17888,9 @@
       <c r="AC318" s="1">
         <v>258</v>
       </c>
+      <c r="AD318" s="25" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="319" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A319" s="34"/>
@@ -18395,6 +18455,27 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="P2:P261"/>
+    <mergeCell ref="P262:P330"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="S2:S261"/>
+    <mergeCell ref="S262:S330"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="J2:J261"/>
+    <mergeCell ref="J262:J330"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="M2:M261"/>
+    <mergeCell ref="M262:M330"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G2:G261"/>
+    <mergeCell ref="G262:G330"/>
+    <mergeCell ref="A2:A261"/>
+    <mergeCell ref="A262:A330"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D2:D261"/>
+    <mergeCell ref="D262:D330"/>
     <mergeCell ref="AB1:AD1"/>
     <mergeCell ref="AB2:AB261"/>
     <mergeCell ref="AB262:AB330"/>
@@ -18404,27 +18485,6 @@
     <mergeCell ref="Y1:AA1"/>
     <mergeCell ref="Y2:Y261"/>
     <mergeCell ref="Y262:Y330"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="G2:G261"/>
-    <mergeCell ref="G262:G330"/>
-    <mergeCell ref="A2:A261"/>
-    <mergeCell ref="A262:A330"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="D2:D261"/>
-    <mergeCell ref="D262:D330"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="J2:J261"/>
-    <mergeCell ref="J262:J330"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="M2:M261"/>
-    <mergeCell ref="M262:M330"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="P2:P261"/>
-    <mergeCell ref="P262:P330"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="S2:S261"/>
-    <mergeCell ref="S262:S330"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>